<commit_message>
from v0.1 to v0.2
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GTP-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GTP-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="76">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -41,7 +41,7 @@
     <t>Reduced (Greedy Heuristic - Transition Pair Coverage)</t>
   </si>
   <si>
-    <t>Size: 7 test case(s))</t>
+    <t>Size: 6 test case(s))</t>
   </si>
   <si>
     <t xml:space="preserve">Creation Date: </t>
@@ -92,6 +92,96 @@
     <t>Actual Result</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - dentro do estado (intermunicipal)</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário NÃO Escolhe o estado.</t>
+  </si>
+  <si>
+    <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Escolhe o tipo de viagem nacional - fora do estado (interestadual).</t>
   </si>
   <si>
@@ -104,139 +194,40 @@
     <t>SYSTEM Exibe a opcao escolhida: estado.</t>
   </si>
   <si>
-    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
-  </si>
-  <si>
     <t>Chefe/Beneficiário Informa as datas de afastamento ALTERNADAS, antes do ultimo dia de viagem.</t>
   </si>
   <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa que acompanha autoridade</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: acompanha autoridade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - dentro do estado (intermunicipal)</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário NÃO Escolhe o estado.</t>
-  </si>
-  <si>
-    <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
+    <t>Chefe/Beneficiário Clica em limpar campos.</t>
+  </si>
+  <si>
+    <t>SYSTEM Apaga todas as seleções do usuário.</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
   </si>
   <si>
     <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
   </si>
   <si>
-    <t>SYSTEM Exibe a opcao escolhida: NÃO acompanha autoridade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em limpar campos.</t>
-  </si>
-  <si>
-    <t>SYSTEM Apaga todas as seleções do usuário.</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
-  </si>
-  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
   </si>
   <si>
     <t>TC4</t>
   </si>
   <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG206 - A categoria funcional do servidor não permite acompanhar autoridades.</t>
+    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
   </si>
   <si>
     <t>TC5</t>
@@ -246,12 +237,6 @@
   </si>
   <si>
     <t>TC6</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
-  </si>
-  <si>
-    <t>TC7</t>
   </si>
   <si>
     <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
@@ -450,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -831,13 +816,13 @@
         <v>12.0</v>
       </c>
       <c r="B21" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s" s="7">
         <v>48</v>
-      </c>
-      <c r="C21" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s" s="7">
-        <v>49</v>
       </c>
       <c r="E21" t="s" s="6">
         <v>2</v>
@@ -851,7 +836,7 @@
         <v>13.0</v>
       </c>
       <c r="B22" t="s" s="7">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s" s="6">
         <v>2</v>
@@ -887,130 +872,130 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n" s="10">
-        <v>15.0</v>
-      </c>
-      <c r="B24" t="s" s="7">
+      <c r="A24" t="s" s="8">
         <v>53</v>
       </c>
-      <c r="C24" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s" s="7">
+      <c r="B24" t="s" s="8">
         <v>54</v>
       </c>
-      <c r="E24" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="8">
+      <c r="C24" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27">
+      <c r="A27" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s" s="4">
         <v>55</v>
       </c>
-      <c r="B25" t="s" s="8">
+      <c r="C27" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F28" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E30" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F30" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B31" t="s" s="7">
         <v>56</v>
       </c>
-      <c r="C25" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F25" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28">
-      <c r="A28" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B28" t="s" s="4">
+      <c r="C31" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s" s="7">
         <v>57</v>
       </c>
-      <c r="C28" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D28" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F28" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B29" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F29" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B30" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F30" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D31" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E31" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F31" t="s" s="5">
-        <v>25</v>
+      <c r="E31" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B32" t="s" s="7">
         <v>58</v>
@@ -1030,16 +1015,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n" s="10">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B33" t="s" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D33" t="s" s="7">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s" s="6">
         <v>2</v>
@@ -1050,16 +1035,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n" s="10">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B34" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D34" t="s" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s" s="6">
         <v>2</v>
@@ -1070,16 +1055,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n" s="10">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B35" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D35" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s" s="6">
         <v>2</v>
@@ -1090,16 +1075,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n" s="10">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B36" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D36" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E36" t="s" s="6">
         <v>2</v>
@@ -1110,16 +1095,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n" s="10">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B37" t="s" s="7">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D37" t="s" s="7">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s" s="6">
         <v>2</v>
@@ -1130,16 +1115,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n" s="10">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D38" t="s" s="7">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s" s="6">
         <v>2</v>
@@ -1150,16 +1135,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n" s="10">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D39" t="s" s="7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s" s="6">
         <v>2</v>
@@ -1170,16 +1155,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n" s="10">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B40" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D40" t="s" s="7">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s" s="6">
         <v>2</v>
@@ -1190,16 +1175,16 @@
     </row>
     <row r="41">
       <c r="A41" t="n" s="10">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B41" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D41" t="s" s="7">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s" s="6">
         <v>2</v>
@@ -1210,7 +1195,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n" s="10">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B42" t="s" s="7">
         <v>46</v>
@@ -1219,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="D42" t="s" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E42" t="s" s="6">
         <v>2</v>
@@ -1230,16 +1215,16 @@
     </row>
     <row r="43">
       <c r="A43" t="n" s="10">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="B43" t="s" s="7">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D43" t="s" s="7">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E43" t="s" s="6">
         <v>2</v>
@@ -1248,140 +1233,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B44" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C44" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s" s="7">
-        <v>50</v>
-      </c>
-      <c r="E44" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F44" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n" s="10">
-        <v>14.0</v>
-      </c>
-      <c r="B45" t="s" s="7">
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s" s="4">
+        <v>63</v>
+      </c>
+      <c r="C46" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F47" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C49" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F49" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B50" t="s" s="7">
         <v>64</v>
       </c>
-      <c r="C45" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s" s="7">
+      <c r="C50" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s" s="7">
         <v>65</v>
       </c>
-      <c r="E45" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F45" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48">
-      <c r="A48" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s" s="4">
+      <c r="E50" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F50" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B51" t="s" s="7">
         <v>66</v>
       </c>
-      <c r="C48" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D48" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E48" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F48" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B49" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C49" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E49" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F49" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B50" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C50" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E50" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F50" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B51" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C51" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D51" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E51" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F51" t="s" s="5">
-        <v>25</v>
+      <c r="C51" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="E51" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n" s="10">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B52" t="s" s="7">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D52" t="s" s="7">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="E52" t="s" s="6">
         <v>2</v>
@@ -1392,16 +1377,16 @@
     </row>
     <row r="53">
       <c r="A53" t="n" s="10">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B53" t="s" s="7">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C53" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D53" t="s" s="7">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E53" t="s" s="6">
         <v>2</v>
@@ -1412,16 +1397,16 @@
     </row>
     <row r="54">
       <c r="A54" t="n" s="10">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="B54" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D54" t="s" s="7">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E54" t="s" s="6">
         <v>2</v>
@@ -1432,16 +1417,16 @@
     </row>
     <row r="55">
       <c r="A55" t="n" s="10">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D55" t="s" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E55" t="s" s="6">
         <v>2</v>
@@ -1452,16 +1437,16 @@
     </row>
     <row r="56">
       <c r="A56" t="n" s="10">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="B56" t="s" s="7">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D56" t="s" s="7">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E56" t="s" s="6">
         <v>2</v>
@@ -1472,16 +1457,16 @@
     </row>
     <row r="57">
       <c r="A57" t="n" s="10">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="B57" t="s" s="7">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C57" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D57" t="s" s="7">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E57" t="s" s="6">
         <v>2</v>
@@ -1492,16 +1477,16 @@
     </row>
     <row r="58">
       <c r="A58" t="n" s="10">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="B58" t="s" s="7">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C58" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D58" t="s" s="7">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E58" t="s" s="6">
         <v>2</v>
@@ -1512,16 +1497,16 @@
     </row>
     <row r="59">
       <c r="A59" t="n" s="10">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="B59" t="s" s="7">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C59" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D59" t="s" s="7">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E59" t="s" s="6">
         <v>2</v>
@@ -1532,16 +1517,16 @@
     </row>
     <row r="60">
       <c r="A60" t="n" s="10">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="B60" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D60" t="s" s="7">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E60" t="s" s="6">
         <v>2</v>
@@ -1552,16 +1537,16 @@
     </row>
     <row r="61">
       <c r="A61" t="n" s="10">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B61" t="s" s="7">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C61" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D61" t="s" s="7">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="E61" t="s" s="6">
         <v>2</v>
@@ -1570,160 +1555,160 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B62" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C62" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D62" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E62" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F62" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B63" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C63" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D63" t="s" s="7">
-        <v>50</v>
-      </c>
-      <c r="E63" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F63" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="62"/>
+    <row r="63"/>
     <row r="64">
-      <c r="A64" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B64" t="s" s="7">
-        <v>51</v>
-      </c>
-      <c r="C64" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="7">
-        <v>72</v>
-      </c>
-      <c r="E64" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F64" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65"/>
-    <row r="66"/>
+      <c r="A64" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s" s="4">
+        <v>70</v>
+      </c>
+      <c r="C64" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D64" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B66" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F66" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
     <row r="67">
-      <c r="A67" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B67" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="C67" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D67" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E67" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F67" t="s" s="4">
-        <v>2</v>
+      <c r="A67" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D67" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E67" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F67" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B68" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C68" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D68" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E68" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F68" t="s" s="9">
+      <c r="A68" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B68" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C68" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E68" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F68" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B69" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C69" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D69" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E69" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F69" t="s" s="8">
+      <c r="A69" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B69" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="C69" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="E69" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F69" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B70" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C70" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D70" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E70" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F70" t="s" s="5">
-        <v>25</v>
+      <c r="A70" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B70" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C70" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E70" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F70" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1734,16 +1719,16 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="E72" t="s" s="6">
         <v>2</v>
@@ -1754,16 +1739,16 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E73" t="s" s="6">
         <v>2</v>
@@ -1774,16 +1759,16 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C74" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E74" t="s" s="6">
         <v>2</v>
@@ -1794,16 +1779,16 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="B75" t="s" s="7">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C75" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E75" t="s" s="6">
         <v>2</v>
@@ -1814,16 +1799,16 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1834,16 +1819,16 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C77" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1854,16 +1839,16 @@
     </row>
     <row r="78">
       <c r="A78" t="n" s="10">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
       <c r="B78" t="s" s="7">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C78" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D78" t="s" s="7">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="E78" t="s" s="6">
         <v>2</v>
@@ -1872,120 +1857,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79"/>
+    <row r="79">
+      <c r="A79" t="n" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="B79" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="E79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F79" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="80"/>
-    <row r="81">
-      <c r="A81" t="s" s="4">
+    <row r="81"/>
+    <row r="82">
+      <c r="A82" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B81" t="s" s="4">
-        <v>75</v>
-      </c>
-      <c r="C81" t="s" s="4">
+      <c r="B82" t="s" s="4">
+        <v>72</v>
+      </c>
+      <c r="C82" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D81" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E81" t="s" s="4">
+      <c r="D82" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F81" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="9">
+      <c r="F82" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B82" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C82" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="9">
+      <c r="B83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F82" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="8">
+      <c r="F83" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B83" t="s" s="8">
+      <c r="B84" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C83" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F83" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s" s="5">
+      <c r="C84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B84" t="s" s="5">
+      <c r="B85" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C84" t="s" s="5">
+      <c r="C85" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D84" t="s" s="5">
+      <c r="D85" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E84" t="s" s="5">
+      <c r="E85" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F84" t="s" s="5">
+      <c r="F85" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B85" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="C85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s" s="7">
-        <v>59</v>
-      </c>
-      <c r="E85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F85" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1996,16 +1981,16 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -2016,16 +2001,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2036,16 +2021,16 @@
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2056,16 +2041,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2076,16 +2061,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2096,16 +2081,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2116,16 +2101,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2136,16 +2121,16 @@
     </row>
     <row r="94">
       <c r="A94" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2156,16 +2141,16 @@
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C95" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2176,16 +2161,16 @@
     </row>
     <row r="96">
       <c r="A96" t="n" s="10">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B96" t="s" s="7">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C96" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E96" t="s" s="6">
         <v>2</v>
@@ -2196,16 +2181,16 @@
     </row>
     <row r="97">
       <c r="A97" t="n" s="10">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="B97" t="s" s="7">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C97" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D97" t="s" s="7">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E97" t="s" s="6">
         <v>2</v>
@@ -2221,7 +2206,7 @@
         <v>12</v>
       </c>
       <c r="B100" t="s" s="4">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C100" t="s" s="4">
         <v>14</v>
@@ -2301,13 +2286,13 @@
         <v>1.0</v>
       </c>
       <c r="B104" t="s" s="7">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C104" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E104" t="s" s="6">
         <v>2</v>
@@ -2321,360 +2306,18 @@
         <v>2.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D105" t="s" s="7">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="F105" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B106" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C106" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D106" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E106" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F106" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B107" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C107" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D107" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E107" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F107" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B108" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C108" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D108" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E108" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F108" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B109" t="s" s="7">
-        <v>71</v>
-      </c>
-      <c r="C109" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D109" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E109" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F109" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B110" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C110" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D110" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E110" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F110" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B111" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C111" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D111" t="s" s="7">
-        <v>63</v>
-      </c>
-      <c r="E111" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F111" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B112" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C112" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D112" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E112" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F112" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B113" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C113" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D113" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E113" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F113" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B114" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C114" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D114" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E114" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F114" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B115" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C115" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D115" t="s" s="7">
-        <v>50</v>
-      </c>
-      <c r="E115" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F115" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B116" t="s" s="7">
-        <v>51</v>
-      </c>
-      <c r="C116" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D116" t="s" s="7">
-        <v>78</v>
-      </c>
-      <c r="E116" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F116" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119">
-      <c r="A119" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B119" t="s" s="4">
-        <v>79</v>
-      </c>
-      <c r="C119" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D119" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E119" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F119" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B120" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C120" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D120" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E120" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F120" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B121" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C121" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D121" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E121" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F121" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B122" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C122" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D122" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E122" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F122" t="s" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B123" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C123" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D123" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="E123" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F123" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B124" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C124" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D124" t="s" s="7">
-        <v>80</v>
-      </c>
-      <c r="E124" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F124" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -2683,19 +2326,17 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:F84"/>
     <mergeCell ref="B101:D101"/>
     <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B120:D120"/>
-    <mergeCell ref="B121:F121"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>